<commit_message>
Adding scripts related to Case Management Dual Approver
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26105"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26111"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="506" documentId="11_01EA95B8EF9627B555DDBF1DCD2D2832789DD15F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6579F509-9292-4481-8D6C-7EA0DBAE1724}"/>
+  <xr:revisionPtr revIDLastSave="738" documentId="11_01EA95B8EF9627B555DDBF1DCD2D2832789DD15F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{083590C9-6935-4D2C-8061-A9D6D1CD5A1B}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19395" windowHeight="10395" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="259">
   <si>
     <t>TCID</t>
   </si>
@@ -151,6 +151,30 @@
     <t>CheckCustodianNotDisplayUntillApproved_Test</t>
   </si>
   <si>
+    <t>VerifyApprovingCaseDualApprovalTypeBothApproved_Test</t>
+  </si>
+  <si>
+    <t>VerifyApprovingCaseDualApprovalTypeFirstOneApproved_Test</t>
+  </si>
+  <si>
+    <t>Initiate_AutoProcess_ForRecordUpto_Collection_SmokeTest</t>
+  </si>
+  <si>
+    <t>VerifyApprovingCaseDualApprovalTypeFirstOneRejected_Test</t>
+  </si>
+  <si>
+    <t>VerifyApprovingCaseDualApprovalTypeBothRejected_Test</t>
+  </si>
+  <si>
+    <t>VerifyApprovingCaseDualApprovalLinearTypeBothApproved_Test</t>
+  </si>
+  <si>
+    <t>Sending_Approving_CaseAndCaseScopeItems_ForApproval</t>
+  </si>
+  <si>
+    <t>VerifyApprovingCaseDualApprovalLinearTypeFirstOneApproved_Test</t>
+  </si>
+  <si>
     <t>Browser</t>
   </si>
   <si>
@@ -184,33 +208,81 @@
     <t>case setting template</t>
   </si>
   <si>
-    <t>nmalegam@ligl.io</t>
+    <t>testligl@ligl.io</t>
   </si>
   <si>
     <t>Vertical@123</t>
   </si>
   <si>
-    <t>LeadName</t>
-  </si>
-  <si>
-    <t>Gates</t>
-  </si>
-  <si>
     <t>Entity</t>
   </si>
   <si>
+    <t>CaseType</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>CaseName</t>
+  </si>
+  <si>
+    <t>CaseSetTemp</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>WFT</t>
+  </si>
+  <si>
+    <t>supervuser</t>
+  </si>
+  <si>
+    <t>Vertical^123</t>
+  </si>
+  <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>antitrust</t>
+  </si>
+  <si>
+    <t>plaintiff</t>
+  </si>
+  <si>
+    <t>QA_SmokeTest1</t>
+  </si>
+  <si>
+    <t>casesetting</t>
+  </si>
+  <si>
+    <t>Vertical south corp</t>
+  </si>
+  <si>
+    <t>Vertical south corp facility</t>
+  </si>
+  <si>
+    <t>Case Creation Test</t>
+  </si>
+  <si>
+    <t>WFT-COLLECTION</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>usa</t>
+    <t>Vertical.123</t>
   </si>
   <si>
     <t>vinaysuperuser</t>
   </si>
   <si>
-    <t>CaseName</t>
-  </si>
-  <si>
     <t>Email1</t>
   </si>
   <si>
@@ -307,9 +379,6 @@
     <t>PartyType</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>QA_Auto11k12</t>
   </si>
   <si>
@@ -605,6 +674,143 @@
   </si>
   <si>
     <t>QA_Auto9v5-Batch143</t>
+  </si>
+  <si>
+    <t>USER1</t>
+  </si>
+  <si>
+    <t>Username1</t>
+  </si>
+  <si>
+    <t>Password1</t>
+  </si>
+  <si>
+    <t>USER2</t>
+  </si>
+  <si>
+    <t>SubType</t>
+  </si>
+  <si>
+    <t>AssignedUser1</t>
+  </si>
+  <si>
+    <t>AssignedUser2</t>
+  </si>
+  <si>
+    <t>QA_Auto13k6</t>
+  </si>
+  <si>
+    <t>QA_Auto13k6-Batch01</t>
+  </si>
+  <si>
+    <t>super vuser</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>Pending Approval</t>
+  </si>
+  <si>
+    <t>Status3</t>
+  </si>
+  <si>
+    <t>QA_Auto19v4</t>
+  </si>
+  <si>
+    <t>QA_Auto19v4-Batch01</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>Custodian</t>
+  </si>
+  <si>
+    <t>DataSource</t>
+  </si>
+  <si>
+    <t>CollectionStatus</t>
+  </si>
+  <si>
+    <t>QA_JAN_23_Case_18</t>
+  </si>
+  <si>
+    <t>Lisa Gang</t>
+  </si>
+  <si>
+    <t>Collection Completed</t>
+  </si>
+  <si>
+    <t>QA_Auto19v5</t>
+  </si>
+  <si>
+    <t>QA_Auto19v5-Batch01</t>
+  </si>
+  <si>
+    <t>QA_Auto20v1</t>
+  </si>
+  <si>
+    <t>QA_Auto20v1-Batch01</t>
+  </si>
+  <si>
+    <t>GmailCheck</t>
+  </si>
+  <si>
+    <t>GoogleDriveCheck</t>
+  </si>
+  <si>
+    <t>QA_Auto20v7</t>
+  </si>
+  <si>
+    <t>Gmail(Not-initiated)</t>
+  </si>
+  <si>
+    <t>Google Drive(Not-initiated)</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>QA_Auto20v7-Batch01</t>
+  </si>
+  <si>
+    <t>CustodianMail</t>
+  </si>
+  <si>
+    <t>BatchName</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>EmailTemp</t>
+  </si>
+  <si>
+    <t>QA_SmokeTest3</t>
+  </si>
+  <si>
+    <t>lisa.gang@verticaldiscovery.us</t>
+  </si>
+  <si>
+    <t>Batch_01</t>
+  </si>
+  <si>
+    <t>0808CaseApproval's Parameters
+0808CaseApproval's Parameters
+CaseApproval</t>
+  </si>
+  <si>
+    <t>QA_SmokeTest3-Batch_01</t>
+  </si>
+  <si>
+    <t>QA_Auto20v8</t>
+  </si>
+  <si>
+    <t>QA_Auto20v8-Batch01</t>
   </si>
 </sst>
 </file>
@@ -717,7 +923,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -733,6 +939,11 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1020,15 +1231,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+    <col min="1" max="1" width="64.28515625" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1325,6 +1536,70 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15">
+      <c r="A38" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1336,180 +1611,261 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O143"/>
+  <dimension ref="A1:AB175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
+    <sheetView tabSelected="1" topLeftCell="Q168" workbookViewId="0">
+      <selection activeCell="W177" sqref="W177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="38.85546875" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" customWidth="1"/>
-    <col min="9" max="9" width="42.28515625" customWidth="1"/>
-    <col min="10" max="10" width="24" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
     <col min="13" max="13" width="21.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" customWidth="1"/>
+    <col min="15" max="15" width="23" customWidth="1"/>
+    <col min="16" max="16" width="28.140625" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="22.85546875" customWidth="1"/>
+    <col min="19" max="19" width="20.85546875" customWidth="1"/>
+    <col min="20" max="20" width="19.140625" customWidth="1"/>
+    <col min="21" max="21" width="16.42578125" customWidth="1"/>
+    <col min="22" max="22" width="20.140625" customWidth="1"/>
+    <col min="23" max="23" width="24.140625" customWidth="1"/>
+    <col min="24" max="24" width="18" customWidth="1"/>
+    <col min="25" max="25" width="25.28515625" customWidth="1"/>
+    <col min="27" max="27" width="21.85546875" customWidth="1"/>
+    <col min="28" max="28" width="19.140625" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" customWidth="1"/>
+    <col min="30" max="30" width="16" customWidth="1"/>
+    <col min="31" max="31" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:14">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>78</v>
+      </c>
+      <c r="N11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1522,16 +1878,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1539,39 +1895,39 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="15"/>
+      <c r="B21" s="18"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1579,16 +1935,16 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1601,16 +1957,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1618,39 +1974,39 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="16"/>
+      <c r="B29" s="19"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1658,40 +2014,40 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1699,41 +2055,41 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D35" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E35" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1741,41 +2097,41 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E39" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1783,1144 +2139,1144 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E43" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E47" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F47" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="H47" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-    </row>
-    <row r="50" spans="1:11" ht="15">
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="H50" s="12" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="J50" s="8"/>
     </row>
-    <row r="51" spans="1:11" ht="15">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D51" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E51" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F51" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="H51" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="I51" s="7"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G54" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="J54" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" t="s">
         <v>71</v>
       </c>
-      <c r="H54" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="I54" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="J54" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="15">
-      <c r="A55" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55" t="s">
-        <v>43</v>
-      </c>
-      <c r="C55" t="s">
-        <v>61</v>
-      </c>
-      <c r="D55" t="s">
-        <v>62</v>
-      </c>
-      <c r="E55" t="s">
-        <v>56</v>
-      </c>
       <c r="F55" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="K58" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="15">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C59" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D59" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E59" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F59" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="H59" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="K59" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="15" t="s">
+      <c r="A61" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B61" s="15"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="15">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" t="s">
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D63" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E63" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F63" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="G63" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="15"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="J66" s="11" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="K66" s="11" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="L66" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="15">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>3</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C67" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D67" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E67" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F67" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="I67" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="J67" s="7" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="K67" s="7" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="L67" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:12">
-      <c r="A69" s="15" t="s">
+      <c r="A69" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B69" s="15"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="I70" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>3</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C71" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D71" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E71" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F71" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="I71" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="15" t="s">
+      <c r="A73" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B73" s="15"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-    </row>
-    <row r="74" spans="1:12" ht="15">
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="K74" s="11" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="L74" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>3</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C75" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D75" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E75" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F75" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="G75" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="I75" s="7" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="J75" t="s">
+        <v>130</v>
+      </c>
+      <c r="K75" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="L75" t="s">
         <v>107</v>
       </c>
-      <c r="K75" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="L75" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" ht="15">
+    </row>
+    <row r="76" spans="1:12">
       <c r="L76" s="7"/>
     </row>
     <row r="77" spans="1:12">
-      <c r="A77" s="15" t="s">
+      <c r="A77" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B77" s="15"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-    </row>
-    <row r="78" spans="1:12" ht="15">
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="H78" s="12" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="I78" s="12" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="J78" s="12" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="K78" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="15">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79" t="s">
         <v>3</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C79" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D79" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E79" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F79" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="G79" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="I79" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="J79" s="7" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="K79" s="7" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="15" t="s">
+      <c r="A81" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B81" s="15"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="J82" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" ht="15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" t="s">
         <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C83" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D83" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E83" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F83" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="H83" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="I83" s="7" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="J83" s="7" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="15" t="s">
+      <c r="A85" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B85" s="15"/>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15"/>
-    </row>
-    <row r="86" spans="1:11" ht="15">
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18"/>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="I86" s="11" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="J86" s="11" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="K86" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" ht="15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87" t="s">
         <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C87" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D87" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E87" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F87" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="H87" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="I87" s="9" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="K87" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="A89" s="15" t="s">
+      <c r="A89" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B89" s="15"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
     </row>
     <row r="90" spans="1:11">
       <c r="A90" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="H90" s="11" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="J90" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" t="s">
         <v>3</v>
       </c>
       <c r="B91" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C91" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D91" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E91" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F91" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="H91" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="I91" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="J91" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:11">
-      <c r="A93" s="15" t="s">
+      <c r="A93" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B93" s="15"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15"/>
+      <c r="B93" s="18"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18"/>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="H94" s="11" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="I94" s="11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" ht="15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95" t="s">
         <v>3</v>
       </c>
       <c r="B95" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C95" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D95" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E95" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F95" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="H95" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="I95" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" ht="15">
-      <c r="A97" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15">
+      <c r="A97" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B97" s="15"/>
-      <c r="C97" s="15"/>
-      <c r="D97" s="15"/>
-    </row>
-    <row r="98" spans="1:15" ht="15">
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+    </row>
+    <row r="98" spans="1:15">
       <c r="A98" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F98" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="H98" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" ht="15">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
         <v>3</v>
       </c>
       <c r="B99" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C99" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D99" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E99" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F99" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="H99" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
     </row>
     <row r="101" spans="1:15">
-      <c r="A101" s="15" t="s">
+      <c r="A101" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B101" s="15"/>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15"/>
+      <c r="B101" s="18"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
     </row>
     <row r="102" spans="1:15">
       <c r="A102" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F102" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G102" s="11" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="H102" s="11" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="I102" s="11" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="J102" s="11" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="K102" s="11" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="L102" s="11" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="M102" s="11" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="N102" s="11" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="O102" s="11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" ht="15">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15">
       <c r="A103" t="s">
         <v>3</v>
       </c>
       <c r="B103" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C103" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D103" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E103" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F103" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="I103" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="K103" s="7" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="L103" s="7" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="M103" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="N103" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="O103" s="7" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
     </row>
     <row r="105" spans="1:15">
-      <c r="A105" s="15" t="s">
+      <c r="A105" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B105" s="15"/>
-      <c r="C105" s="15"/>
-      <c r="D105" s="15"/>
-    </row>
-    <row r="106" spans="1:15" ht="15">
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+    </row>
+    <row r="106" spans="1:15">
       <c r="A106" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F106" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G106" s="11" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="H106" s="10"/>
     </row>
@@ -2929,227 +3285,227 @@
         <v>3</v>
       </c>
       <c r="B107" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C107" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D107" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E107" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F107" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="G107" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
     </row>
     <row r="109" spans="1:15">
-      <c r="A109" s="15" t="s">
+      <c r="A109" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B109" s="15"/>
-      <c r="C109" s="15"/>
-      <c r="D109" s="15"/>
+      <c r="B109" s="18"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="18"/>
     </row>
     <row r="110" spans="1:15">
       <c r="A110" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F110" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G110" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="H110" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="I110" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J110" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="K110" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="H110" s="11" t="s">
+      <c r="L110" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="I110" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="J110" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="K110" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="L110" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" ht="15">
+    </row>
+    <row r="111" spans="1:15">
       <c r="A111" t="s">
         <v>3</v>
       </c>
       <c r="B111" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C111" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D111" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E111" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F111" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
       <c r="G111" t="s">
+        <v>183</v>
+      </c>
+      <c r="H111" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="I111" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H111" s="10" t="s">
+      <c r="J111" t="s">
         <v>161</v>
       </c>
-      <c r="I111" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J111" t="s">
-        <v>138</v>
-      </c>
       <c r="K111" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="L111" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
     </row>
     <row r="113" spans="1:13">
-      <c r="A113" s="15" t="s">
+      <c r="A113" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B113" s="15"/>
-      <c r="C113" s="15"/>
-      <c r="D113" s="15"/>
-    </row>
-    <row r="114" spans="1:13" ht="15">
+      <c r="B113" s="18"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="18"/>
+    </row>
+    <row r="114" spans="1:13">
       <c r="A114" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E114" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F114" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G114" s="11" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="H114" s="11" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="J114" s="11" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="K114" s="14" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="L114" s="11" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="M114" s="11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" ht="15">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13">
       <c r="A115" t="s">
         <v>3</v>
       </c>
       <c r="B115" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C115" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D115" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E115" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F115" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="H115" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="I115" s="9" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="J115" s="9" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="K115" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="L115" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="M115" s="10" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
     </row>
     <row r="117" spans="1:13">
-      <c r="A117" s="15" t="s">
+      <c r="A117" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B117" s="15"/>
-      <c r="C117" s="15"/>
-      <c r="D117" s="15"/>
-    </row>
-    <row r="118" spans="1:13" ht="15">
+      <c r="B117" s="18"/>
+      <c r="C117" s="18"/>
+      <c r="D117" s="18"/>
+    </row>
+    <row r="118" spans="1:13">
       <c r="A118" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F118" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G118" s="14" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="H118" s="7"/>
     </row>
@@ -3158,59 +3514,59 @@
         <v>3</v>
       </c>
       <c r="B119" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C119" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D119" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E119" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F119" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="G119" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
     </row>
     <row r="121" spans="1:13">
-      <c r="A121" s="15" t="s">
+      <c r="A121" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B121" s="15"/>
-      <c r="C121" s="15"/>
-      <c r="D121" s="15"/>
+      <c r="B121" s="18"/>
+      <c r="C121" s="18"/>
+      <c r="D121" s="18"/>
     </row>
     <row r="122" spans="1:13">
       <c r="A122" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G122" s="11" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="H122" s="11" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="I122" s="11" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
       <c r="J122" s="11"/>
     </row>
@@ -3219,56 +3575,56 @@
         <v>3</v>
       </c>
       <c r="B123" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C123" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D123" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E123" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F123" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="G123" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="H123" t="s">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="I123" t="s">
-        <v>172</v>
+        <v>195</v>
       </c>
     </row>
     <row r="125" spans="1:13">
-      <c r="A125" s="15" t="s">
+      <c r="A125" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B125" s="15"/>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
+      <c r="B125" s="18"/>
+      <c r="C125" s="18"/>
+      <c r="D125" s="18"/>
     </row>
     <row r="126" spans="1:13">
       <c r="A126" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F126" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="127" spans="1:13">
@@ -3276,53 +3632,53 @@
         <v>3</v>
       </c>
       <c r="B127" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C127" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D127" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E127" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F127" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
     </row>
     <row r="129" spans="1:13">
-      <c r="A129" s="15" t="s">
+      <c r="A129" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B129" s="15"/>
-      <c r="C129" s="15"/>
-      <c r="D129" s="15"/>
+      <c r="B129" s="18"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="18"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F130" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G130" s="11" t="s">
-        <v>167</v>
+        <v>190</v>
       </c>
       <c r="H130" s="11" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
     </row>
     <row r="131" spans="1:13">
@@ -3330,53 +3686,53 @@
         <v>3</v>
       </c>
       <c r="B131" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C131" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D131" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E131" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F131" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="G131" t="s">
-        <v>176</v>
+        <v>199</v>
       </c>
       <c r="H131" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="1:13">
-      <c r="A133" s="15" t="s">
+      <c r="A133" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B133" s="15"/>
-      <c r="C133" s="15"/>
-      <c r="D133" s="15"/>
+      <c r="B133" s="18"/>
+      <c r="C133" s="18"/>
+      <c r="D133" s="18"/>
     </row>
     <row r="134" spans="1:13">
       <c r="A134" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F134" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="135" spans="1:13">
@@ -3384,59 +3740,59 @@
         <v>3</v>
       </c>
       <c r="B135" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C135" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D135" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E135" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F135" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
     </row>
     <row r="137" spans="1:13">
-      <c r="A137" s="15" t="s">
+      <c r="A137" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B137" s="15"/>
-      <c r="C137" s="15"/>
-      <c r="D137" s="15"/>
+      <c r="B137" s="18"/>
+      <c r="C137" s="18"/>
+      <c r="D137" s="18"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F138" s="11" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G138" s="11" t="s">
-        <v>178</v>
+        <v>201</v>
       </c>
       <c r="H138" s="11" t="s">
-        <v>179</v>
+        <v>202</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="J138" s="11" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
     </row>
     <row r="139" spans="1:13">
@@ -3444,141 +3800,1203 @@
         <v>3</v>
       </c>
       <c r="B139" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C139" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D139" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="E139" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F139" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="G139" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="H139" t="s">
-        <v>183</v>
+        <v>206</v>
       </c>
       <c r="I139" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="J139" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
     </row>
     <row r="141" spans="1:13">
-      <c r="A141" s="15" t="s">
+      <c r="A141" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B141" s="15"/>
-      <c r="C141" s="15"/>
-      <c r="D141" s="15"/>
+      <c r="B141" s="18"/>
+      <c r="C141" s="18"/>
+      <c r="D141" s="18"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B142" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F142" t="s">
+        <v>63</v>
+      </c>
+      <c r="G142" t="s">
+        <v>83</v>
+      </c>
+      <c r="H142" t="s">
+        <v>147</v>
+      </c>
+      <c r="I142" t="s">
+        <v>209</v>
+      </c>
+      <c r="J142" t="s">
+        <v>201</v>
+      </c>
+      <c r="K142" t="s">
+        <v>202</v>
+      </c>
+      <c r="L142" t="s">
+        <v>203</v>
+      </c>
+      <c r="M142" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13">
+      <c r="A143" t="s">
+        <v>3</v>
+      </c>
+      <c r="B143" t="s">
+        <v>51</v>
+      </c>
+      <c r="C143" t="s">
+        <v>85</v>
+      </c>
+      <c r="D143" t="s">
+        <v>86</v>
+      </c>
+      <c r="E143" t="s">
+        <v>71</v>
+      </c>
+      <c r="F143" t="s">
+        <v>210</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H143" t="s">
+        <v>89</v>
+      </c>
+      <c r="I143" t="s">
+        <v>211</v>
+      </c>
+      <c r="J143" t="s">
+        <v>212</v>
+      </c>
+      <c r="K143" t="s">
+        <v>206</v>
+      </c>
+      <c r="L143" t="s">
+        <v>207</v>
+      </c>
+      <c r="M143" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="145" spans="1:21">
+      <c r="A145" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="B145" s="18"/>
+      <c r="C145" s="18"/>
+      <c r="D145" s="18"/>
+    </row>
+    <row r="146" spans="1:21">
+      <c r="A146" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E146" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F146" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G146" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="H146" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I146" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J146" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="K146" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L146" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M146" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="N146" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="O146" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="P146" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q146" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="R146" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="S146" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="T146" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="147" spans="1:21">
+      <c r="A147" t="s">
+        <v>3</v>
+      </c>
+      <c r="B147" t="s">
+        <v>51</v>
+      </c>
+      <c r="C147" t="s">
+        <v>85</v>
+      </c>
+      <c r="D147" t="s">
+        <v>86</v>
+      </c>
+      <c r="E147" t="s">
+        <v>71</v>
+      </c>
+      <c r="F147" t="s">
+        <v>221</v>
+      </c>
+      <c r="G147" t="s">
+        <v>205</v>
+      </c>
+      <c r="H147" t="s">
+        <v>206</v>
+      </c>
+      <c r="I147" t="s">
+        <v>207</v>
+      </c>
+      <c r="J147" t="s">
+        <v>222</v>
+      </c>
+      <c r="K147" t="s">
+        <v>69</v>
+      </c>
+      <c r="L147" t="s">
+        <v>70</v>
+      </c>
+      <c r="M147" t="s">
+        <v>223</v>
+      </c>
+      <c r="N147" t="s">
+        <v>89</v>
+      </c>
+      <c r="O147" t="s">
+        <v>224</v>
+      </c>
+      <c r="P147" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q147" t="s">
+        <v>85</v>
+      </c>
+      <c r="R147" t="s">
+        <v>225</v>
+      </c>
+      <c r="S147" t="s">
+        <v>69</v>
+      </c>
+      <c r="T147" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="149" spans="1:21" ht="15" customHeight="1">
+      <c r="A149" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D142" s="2" t="s">
+      <c r="B149" s="18"/>
+      <c r="C149" s="18"/>
+      <c r="D149" s="18"/>
+    </row>
+    <row r="150" spans="1:21" ht="15" customHeight="1">
+      <c r="A150" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E150" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F150" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G150" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="H150" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I150" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J150" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="K150" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L150" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M150" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="N150" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="O150" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="P150" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q150" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="R150" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="S150" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="T150" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="U150" s="15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="151" spans="1:21" ht="15" customHeight="1">
+      <c r="A151" t="s">
+        <v>3</v>
+      </c>
+      <c r="B151" t="s">
+        <v>51</v>
+      </c>
+      <c r="C151" t="s">
+        <v>85</v>
+      </c>
+      <c r="D151" t="s">
+        <v>86</v>
+      </c>
+      <c r="E151" t="s">
+        <v>71</v>
+      </c>
+      <c r="F151" t="s">
+        <v>228</v>
+      </c>
+      <c r="G151" t="s">
+        <v>205</v>
+      </c>
+      <c r="H151" t="s">
+        <v>206</v>
+      </c>
+      <c r="I151" t="s">
+        <v>207</v>
+      </c>
+      <c r="J151" t="s">
+        <v>229</v>
+      </c>
+      <c r="K151" t="s">
+        <v>69</v>
+      </c>
+      <c r="L151" t="s">
+        <v>70</v>
+      </c>
+      <c r="M151" t="s">
+        <v>223</v>
+      </c>
+      <c r="N151" t="s">
+        <v>89</v>
+      </c>
+      <c r="O151" t="s">
+        <v>224</v>
+      </c>
+      <c r="P151" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q151" t="s">
+        <v>85</v>
+      </c>
+      <c r="R151" t="s">
+        <v>225</v>
+      </c>
+      <c r="S151" t="s">
+        <v>69</v>
+      </c>
+      <c r="T151" t="s">
+        <v>226</v>
+      </c>
+      <c r="U151" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="153" spans="1:21" ht="15" customHeight="1">
+      <c r="A153" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E142" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F142" t="s">
-        <v>58</v>
-      </c>
-      <c r="G142" t="s">
-        <v>59</v>
-      </c>
-      <c r="H142" t="s">
-        <v>124</v>
-      </c>
-      <c r="I142" t="s">
+      <c r="B153" s="4"/>
+      <c r="C153" s="4"/>
+      <c r="D153" s="4"/>
+    </row>
+    <row r="154" spans="1:21" ht="15" customHeight="1">
+      <c r="A154" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F154" t="s">
+        <v>63</v>
+      </c>
+      <c r="G154" t="s">
+        <v>231</v>
+      </c>
+      <c r="H154" t="s">
+        <v>232</v>
+      </c>
+      <c r="I154" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="155" spans="1:21" ht="15" customHeight="1">
+      <c r="A155" t="s">
+        <v>3</v>
+      </c>
+      <c r="B155" t="s">
+        <v>51</v>
+      </c>
+      <c r="C155" t="s">
+        <v>69</v>
+      </c>
+      <c r="D155" t="s">
+        <v>70</v>
+      </c>
+      <c r="E155" t="s">
+        <v>71</v>
+      </c>
+      <c r="F155" t="s">
+        <v>234</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H155" t="s">
+        <v>163</v>
+      </c>
+      <c r="I155" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="157" spans="1:21" ht="15" customHeight="1">
+      <c r="A157" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B157" s="18"/>
+      <c r="C157" s="18"/>
+      <c r="D157" s="18"/>
+    </row>
+    <row r="158" spans="1:21" ht="15" customHeight="1">
+      <c r="A158" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E158" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F158" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G158" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="H158" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I158" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J158" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="J142" t="s">
-        <v>178</v>
-      </c>
-      <c r="K142" t="s">
-        <v>179</v>
-      </c>
-      <c r="L142" t="s">
+      <c r="K158" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L158" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M158" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="N158" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="O158" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="P158" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q158" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="R158" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="M142" t="s">
+      <c r="S158" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="T158" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="U158" s="15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21" ht="15" customHeight="1">
+      <c r="A159" t="s">
+        <v>3</v>
+      </c>
+      <c r="B159" t="s">
+        <v>51</v>
+      </c>
+      <c r="C159" t="s">
+        <v>85</v>
+      </c>
+      <c r="D159" t="s">
+        <v>86</v>
+      </c>
+      <c r="E159" t="s">
+        <v>71</v>
+      </c>
+      <c r="F159" t="s">
+        <v>237</v>
+      </c>
+      <c r="G159" t="s">
+        <v>205</v>
+      </c>
+      <c r="H159" t="s">
+        <v>206</v>
+      </c>
+      <c r="I159" t="s">
+        <v>207</v>
+      </c>
+      <c r="J159" t="s">
+        <v>238</v>
+      </c>
+      <c r="K159" t="s">
+        <v>69</v>
+      </c>
+      <c r="L159" t="s">
+        <v>70</v>
+      </c>
+      <c r="M159" t="s">
+        <v>223</v>
+      </c>
+      <c r="N159" t="s">
+        <v>89</v>
+      </c>
+      <c r="O159" t="s">
+        <v>224</v>
+      </c>
+      <c r="P159" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q159" t="s">
+        <v>85</v>
+      </c>
+      <c r="R159" t="s">
+        <v>225</v>
+      </c>
+      <c r="S159" t="s">
+        <v>69</v>
+      </c>
+      <c r="T159" t="s">
+        <v>226</v>
+      </c>
+      <c r="U159" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="161" spans="1:28" ht="15" customHeight="1">
+      <c r="A161" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B161" s="18"/>
+      <c r="C161" s="18"/>
+      <c r="D161" s="18"/>
+    </row>
+    <row r="162" spans="1:28" ht="15" customHeight="1">
+      <c r="A162" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E162" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F162" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G162" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="H162" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="I162" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J162" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="K162" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L162" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="M162" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="N162" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="O162" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="P162" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q162" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="R162" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="S162" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="T162" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="U162" s="15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="163" spans="1:28" ht="15" customHeight="1">
+      <c r="A163" t="s">
+        <v>3</v>
+      </c>
+      <c r="B163" t="s">
+        <v>51</v>
+      </c>
+      <c r="C163" t="s">
+        <v>85</v>
+      </c>
+      <c r="D163" t="s">
+        <v>86</v>
+      </c>
+      <c r="E163" t="s">
+        <v>71</v>
+      </c>
+      <c r="F163" t="s">
+        <v>239</v>
+      </c>
+      <c r="G163" t="s">
+        <v>205</v>
+      </c>
+      <c r="H163" t="s">
+        <v>206</v>
+      </c>
+      <c r="I163" t="s">
+        <v>207</v>
+      </c>
+      <c r="J163" t="s">
+        <v>240</v>
+      </c>
+      <c r="K163" t="s">
+        <v>69</v>
+      </c>
+      <c r="L163" t="s">
+        <v>70</v>
+      </c>
+      <c r="M163" t="s">
+        <v>223</v>
+      </c>
+      <c r="N163" t="s">
+        <v>89</v>
+      </c>
+      <c r="O163" t="s">
+        <v>224</v>
+      </c>
+      <c r="P163" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q163" t="s">
+        <v>85</v>
+      </c>
+      <c r="R163" t="s">
+        <v>225</v>
+      </c>
+      <c r="S163" t="s">
+        <v>69</v>
+      </c>
+      <c r="T163" t="s">
+        <v>226</v>
+      </c>
+      <c r="U163" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="165" spans="1:28" ht="15" customHeight="1">
+      <c r="A165" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B165" s="18"/>
+      <c r="C165" s="18"/>
+      <c r="D165" s="18"/>
+    </row>
+    <row r="166" spans="1:28" ht="15" customHeight="1">
+      <c r="A166" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E166" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F166" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G166" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H166" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I166" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="J166" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="K166" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="L166" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="M166" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="N166" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="O166" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="P166" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q166" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="R166" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="S166" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="T166" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="U166" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="V166" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="W166" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="X166" s="11"/>
+      <c r="Y166" s="11"/>
+      <c r="Z166" s="11"/>
+      <c r="AA166" s="11"/>
+      <c r="AB166" s="11"/>
+    </row>
+    <row r="167" spans="1:28" ht="15" customHeight="1">
+      <c r="A167" t="s">
+        <v>3</v>
+      </c>
+      <c r="B167" t="s">
+        <v>51</v>
+      </c>
+      <c r="C167" t="s">
+        <v>85</v>
+      </c>
+      <c r="D167" t="s">
+        <v>86</v>
+      </c>
+      <c r="E167" t="s">
+        <v>71</v>
+      </c>
+      <c r="F167" t="s">
+        <v>243</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H167" t="s">
+        <v>89</v>
+      </c>
+      <c r="I167" t="s">
+        <v>244</v>
+      </c>
+      <c r="J167" t="s">
+        <v>245</v>
+      </c>
+      <c r="K167" t="s">
+        <v>205</v>
+      </c>
+      <c r="L167" t="s">
+        <v>206</v>
+      </c>
+      <c r="M167" t="s">
+        <v>223</v>
+      </c>
+      <c r="N167" t="s">
+        <v>246</v>
+      </c>
+      <c r="O167" t="s">
+        <v>207</v>
+      </c>
+      <c r="P167" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q167" t="s">
+        <v>69</v>
+      </c>
+      <c r="R167" t="s">
+        <v>70</v>
+      </c>
+      <c r="S167" t="s">
+        <v>85</v>
+      </c>
+      <c r="T167" t="s">
+        <v>225</v>
+      </c>
+      <c r="U167" t="s">
+        <v>69</v>
+      </c>
+      <c r="V167" t="s">
+        <v>226</v>
+      </c>
+      <c r="W167" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB167" s="1"/>
+    </row>
+    <row r="169" spans="1:28" ht="15" customHeight="1">
+      <c r="A169" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B169" s="4"/>
+      <c r="C169" s="4"/>
+    </row>
+    <row r="170" spans="1:28" ht="15" customHeight="1">
+      <c r="A170" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E170" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F170" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G170" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H170" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I170" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J170" t="s">
+        <v>60</v>
+      </c>
+      <c r="K170" t="s">
+        <v>65</v>
+      </c>
+      <c r="L170" t="s">
+        <v>66</v>
+      </c>
+      <c r="M170" t="s">
+        <v>67</v>
+      </c>
+      <c r="N170" t="s">
+        <v>68</v>
+      </c>
+      <c r="O170" t="s">
+        <v>248</v>
+      </c>
+      <c r="P170" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q170" t="s">
+        <v>231</v>
+      </c>
+      <c r="R170" t="s">
+        <v>158</v>
+      </c>
+      <c r="S170" t="s">
+        <v>249</v>
+      </c>
+      <c r="T170" t="s">
+        <v>250</v>
+      </c>
+      <c r="U170" t="s">
+        <v>251</v>
+      </c>
+      <c r="V170" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="171" spans="1:28" ht="15" customHeight="1">
+      <c r="A171" t="s">
+        <v>3</v>
+      </c>
+      <c r="B171" t="s">
+        <v>51</v>
+      </c>
+      <c r="C171" t="s">
+        <v>69</v>
+      </c>
+      <c r="D171" t="s">
+        <v>70</v>
+      </c>
+      <c r="E171" t="s">
+        <v>71</v>
+      </c>
+      <c r="F171" t="s">
+        <v>72</v>
+      </c>
+      <c r="G171" t="s">
+        <v>73</v>
+      </c>
+      <c r="H171" t="s">
+        <v>252</v>
+      </c>
+      <c r="I171" t="s">
+        <v>75</v>
+      </c>
+      <c r="J171" t="s">
+        <v>76</v>
+      </c>
+      <c r="K171" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L171">
+        <v>2</v>
+      </c>
+      <c r="M171" t="s">
+        <v>78</v>
+      </c>
+      <c r="N171" t="s">
+        <v>79</v>
+      </c>
+      <c r="O171" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="P171" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="143" spans="1:13" ht="15">
-      <c r="A143" t="s">
-        <v>3</v>
-      </c>
-      <c r="B143" t="s">
-        <v>43</v>
-      </c>
-      <c r="C143" t="s">
-        <v>61</v>
-      </c>
-      <c r="D143" t="s">
-        <v>62</v>
-      </c>
-      <c r="E143" t="s">
-        <v>56</v>
-      </c>
-      <c r="F143" t="s">
-        <v>187</v>
-      </c>
-      <c r="G143" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H143" t="s">
-        <v>65</v>
-      </c>
-      <c r="I143" t="s">
-        <v>188</v>
-      </c>
-      <c r="J143" t="s">
-        <v>189</v>
-      </c>
-      <c r="K143" t="s">
-        <v>183</v>
-      </c>
-      <c r="L143" t="s">
-        <v>184</v>
-      </c>
-      <c r="M143" t="s">
-        <v>190</v>
+      <c r="Q171" t="s">
+        <v>235</v>
+      </c>
+      <c r="R171" t="s">
+        <v>163</v>
+      </c>
+      <c r="S171" t="s">
+        <v>254</v>
+      </c>
+      <c r="T171" t="s">
+        <v>223</v>
+      </c>
+      <c r="U171" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="V171" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="173" spans="1:28" ht="15" customHeight="1">
+      <c r="A173" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B173" s="18"/>
+      <c r="C173" s="18"/>
+      <c r="D173" s="18"/>
+    </row>
+    <row r="174" spans="1:28" ht="15" customHeight="1">
+      <c r="A174" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E174" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F174" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G174" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H174" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I174" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="J174" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="K174" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="L174" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="M174" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="N174" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="O174" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="P174" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q174" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="R174" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="S174" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="T174" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="U174" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="V174" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="W174" s="15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="175" spans="1:28" ht="15" customHeight="1">
+      <c r="A175" t="s">
+        <v>3</v>
+      </c>
+      <c r="B175" t="s">
+        <v>51</v>
+      </c>
+      <c r="C175" t="s">
+        <v>85</v>
+      </c>
+      <c r="D175" t="s">
+        <v>86</v>
+      </c>
+      <c r="E175" t="s">
+        <v>71</v>
+      </c>
+      <c r="F175" t="s">
+        <v>257</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H175" t="s">
+        <v>89</v>
+      </c>
+      <c r="I175" t="s">
+        <v>244</v>
+      </c>
+      <c r="J175" t="s">
+        <v>245</v>
+      </c>
+      <c r="K175" t="s">
+        <v>205</v>
+      </c>
+      <c r="L175" t="s">
+        <v>206</v>
+      </c>
+      <c r="M175" t="s">
+        <v>223</v>
+      </c>
+      <c r="N175" t="s">
+        <v>246</v>
+      </c>
+      <c r="O175" t="s">
+        <v>207</v>
+      </c>
+      <c r="P175" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q175" t="s">
+        <v>69</v>
+      </c>
+      <c r="R175" t="s">
+        <v>70</v>
+      </c>
+      <c r="S175" t="s">
+        <v>85</v>
+      </c>
+      <c r="T175" t="s">
+        <v>225</v>
+      </c>
+      <c r="U175" t="s">
+        <v>69</v>
+      </c>
+      <c r="V175" t="s">
+        <v>226</v>
+      </c>
+      <c r="W175" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="A141:D141"/>
-    <mergeCell ref="A57:D57"/>
+  <mergeCells count="36">
+    <mergeCell ref="A173:D173"/>
+    <mergeCell ref="A165:D165"/>
+    <mergeCell ref="A81:D81"/>
     <mergeCell ref="A93:D93"/>
     <mergeCell ref="A89:D89"/>
     <mergeCell ref="A85:D85"/>
     <mergeCell ref="A133:D133"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A61:D61"/>
     <mergeCell ref="A105:D105"/>
     <mergeCell ref="A101:D101"/>
     <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="A121:D121"/>
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="A137:D137"/>
+    <mergeCell ref="A141:D141"/>
     <mergeCell ref="A77:D77"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A41:D41"/>
@@ -3588,11 +5006,16 @@
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A161:D161"/>
+    <mergeCell ref="A157:D157"/>
+    <mergeCell ref="A149:D149"/>
+    <mergeCell ref="A145:D145"/>
     <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="A121:D121"/>
-    <mergeCell ref="A117:D117"/>
-    <mergeCell ref="A137:D137"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -3672,9 +5095,47 @@
     <hyperlink ref="D43" r:id="rId75" xr:uid="{9103D47E-17CE-42E4-981F-4D7FF3B84652}"/>
     <hyperlink ref="C43" r:id="rId76" display="nmalegam@ligl.io" xr:uid="{9453F1E1-018D-4EB6-8466-C00DE5CA7A01}"/>
     <hyperlink ref="D59" r:id="rId77" xr:uid="{421CC160-F02A-485E-A8F7-102913010A7E}"/>
+    <hyperlink ref="D147" r:id="rId78" xr:uid="{88A569DE-2718-4522-BF7F-62FB0537E2EC}"/>
+    <hyperlink ref="C147" r:id="rId79" display="nmalegam@ligl.io" xr:uid="{BF026495-E72D-483E-9151-F09DD5D0384A}"/>
+    <hyperlink ref="L147" r:id="rId80" xr:uid="{4ACC9848-EC80-4DFB-8ADB-03380C7A3FD7}"/>
+    <hyperlink ref="K147" r:id="rId81" display="nmalegam@ligl.io" xr:uid="{B7CC252A-8216-4278-9E98-52D3569084DE}"/>
+    <hyperlink ref="P147" r:id="rId82" xr:uid="{7DD83972-22C9-4FC2-9FE4-64A3C1694C32}"/>
+    <hyperlink ref="D151" r:id="rId83" xr:uid="{1B819952-2D42-46B1-B947-987A4E949831}"/>
+    <hyperlink ref="C151" r:id="rId84" display="nmalegam@ligl.io" xr:uid="{ACC1EB0F-A775-4608-B02F-F7AA6BF9567D}"/>
+    <hyperlink ref="L151" r:id="rId85" xr:uid="{CA7CDF56-1E7E-45EE-A5B7-79EE95515E1D}"/>
+    <hyperlink ref="K151" r:id="rId86" display="nmalegam@ligl.io" xr:uid="{427845D7-C689-43C6-89B6-8DC0F0654FD2}"/>
+    <hyperlink ref="P151" r:id="rId87" xr:uid="{F27BCDD9-A04D-41B7-A7CE-5D9B70D6E49D}"/>
+    <hyperlink ref="D155" r:id="rId88" xr:uid="{A21076E0-7F79-4E04-87F0-5A502510B5D1}"/>
+    <hyperlink ref="C155" r:id="rId89" display="nmalegam@ligl.io" xr:uid="{9493ED02-CEA3-4249-95C6-A415D4DD6E50}"/>
+    <hyperlink ref="G155" r:id="rId90" display="vyerra@ligl.io" xr:uid="{D05ABF08-F5DA-4457-8147-45A50B2292E0}"/>
+    <hyperlink ref="D159" r:id="rId91" xr:uid="{B30B9CF8-614B-4B8C-B818-287AAE033FBF}"/>
+    <hyperlink ref="C159" r:id="rId92" display="nmalegam@ligl.io" xr:uid="{6C94F27F-BA6D-4547-B92E-83501793B5BA}"/>
+    <hyperlink ref="L159" r:id="rId93" xr:uid="{FE5A0C61-C6A8-43DE-A460-B97763B8A95D}"/>
+    <hyperlink ref="K159" r:id="rId94" display="nmalegam@ligl.io" xr:uid="{73132630-1EAB-4C01-AE7C-96B2F645B60E}"/>
+    <hyperlink ref="P159" r:id="rId95" xr:uid="{6F92B482-7B5F-41C6-A662-184409BBA568}"/>
+    <hyperlink ref="D163" r:id="rId96" xr:uid="{B03F8876-EF63-4AFE-9574-6BB593A15844}"/>
+    <hyperlink ref="C163" r:id="rId97" display="nmalegam@ligl.io" xr:uid="{DB5BAAF4-AE3A-4C2C-9D69-558368412BF0}"/>
+    <hyperlink ref="L163" r:id="rId98" xr:uid="{8A7E1CA5-921A-426D-827E-E94E18C95FFE}"/>
+    <hyperlink ref="K163" r:id="rId99" display="nmalegam@ligl.io" xr:uid="{857126CC-28CD-410A-9D51-CB114BEA8808}"/>
+    <hyperlink ref="P163" r:id="rId100" xr:uid="{196FE437-4961-45F7-9F9C-C3F54F3C176E}"/>
+    <hyperlink ref="D167" r:id="rId101" xr:uid="{884F1BF6-C051-4ED3-8F89-DEBACBB05112}"/>
+    <hyperlink ref="C167" r:id="rId102" display="nmalegam@ligl.io" xr:uid="{B5630939-E815-4F62-8253-6BF8A538151A}"/>
+    <hyperlink ref="R167" r:id="rId103" xr:uid="{254F85AD-9F92-4534-957D-07DFB8F6D580}"/>
+    <hyperlink ref="Q167" r:id="rId104" display="nmalegam@ligl.io" xr:uid="{90AE60ED-40C9-47F5-A6BF-E48B85976826}"/>
+    <hyperlink ref="C11" r:id="rId105" display="nmalegam@ligl.io" xr:uid="{ABF323FA-7B90-44C1-8D5D-F432051D88C3}"/>
+    <hyperlink ref="D11" r:id="rId106" xr:uid="{ACEF8D99-DE27-42E2-AEC5-C396346ADBF4}"/>
+    <hyperlink ref="G167" r:id="rId107" xr:uid="{7D2536A0-8BFC-42D6-AEC4-F0F3A31A42BB}"/>
+    <hyperlink ref="C171" r:id="rId108" display="nmalegam@ligl.io" xr:uid="{3700B464-823E-4A0A-9528-D30AE8439CBD}"/>
+    <hyperlink ref="D171" r:id="rId109" xr:uid="{20F8FD15-C039-4831-BA5B-4680F0BF4910}"/>
+    <hyperlink ref="O171" r:id="rId110" xr:uid="{1D766624-AAD1-4778-A5B1-63769F263A0B}"/>
+    <hyperlink ref="D175" r:id="rId111" xr:uid="{8A0956B6-D9D4-439E-ACA3-98967207D4AD}"/>
+    <hyperlink ref="C175" r:id="rId112" display="nmalegam@ligl.io" xr:uid="{301744EA-8D42-467A-B0E7-0123A8C20B47}"/>
+    <hyperlink ref="R175" r:id="rId113" xr:uid="{7F47E7F3-0739-4457-AEF8-48CD18B278B0}"/>
+    <hyperlink ref="Q175" r:id="rId114" display="nmalegam@ligl.io" xr:uid="{823E1127-A1B3-4C02-931B-14CDE42A5976}"/>
+    <hyperlink ref="G175" r:id="rId115" xr:uid="{130E9A4A-8C1F-44BD-AA59-D429B5C7F5A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId78"/>
+  <pageSetup orientation="portrait" r:id="rId116"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding smoke Suite And Dual Approval Test Cases
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26111"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="738" documentId="11_01EA95B8EF9627B555DDBF1DCD2D2832789DD15F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{083590C9-6935-4D2C-8061-A9D6D1CD5A1B}"/>
+  <xr:revisionPtr revIDLastSave="813" documentId="11_01EA95B8EF9627B555DDBF1DCD2D2832789DD15F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95D13978-44A4-4A2E-81CB-3CA16B15D48C}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19395" windowHeight="10395" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="263">
   <si>
     <t>TCID</t>
   </si>
@@ -169,7 +169,7 @@
     <t>VerifyApprovingCaseDualApprovalLinearTypeBothApproved_Test</t>
   </si>
   <si>
-    <t>Sending_Approving_CaseAndCaseScopeItems_ForApproval</t>
+    <t>Create_Sending_Approving_CaseAndCaseScopeItems_ForApproval</t>
   </si>
   <si>
     <t>VerifyApprovingCaseDualApprovalLinearTypeFirstOneApproved_Test</t>
@@ -733,15 +733,24 @@
     <t>DataSource</t>
   </si>
   <si>
+    <t>DataHold</t>
+  </si>
+  <si>
     <t>CollectionStatus</t>
   </si>
   <si>
-    <t>QA_JAN_23_Case_18</t>
+    <t>QA_Automation_SmokeSuite27</t>
   </si>
   <si>
     <t>Lisa Gang</t>
   </si>
   <si>
+    <t>Slack</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>Collection Completed</t>
   </si>
   <si>
@@ -790,27 +799,28 @@
     <t>EmailTemp</t>
   </si>
   <si>
-    <t>QA_SmokeTest3</t>
-  </si>
-  <si>
     <t>lisa.gang@verticaldiscovery.us</t>
   </si>
   <si>
+    <t>Slack(Not-initiated)</t>
+  </si>
+  <si>
     <t>Batch_01</t>
   </si>
   <si>
-    <t>0808CaseApproval's Parameters
-0808CaseApproval's Parameters
-CaseApproval</t>
-  </si>
-  <si>
-    <t>QA_SmokeTest3-Batch_01</t>
-  </si>
-  <si>
-    <t>QA_Auto20v8</t>
-  </si>
-  <si>
-    <t>QA_Auto20v8-Batch01</t>
+    <t>TES# L!GL</t>
+  </si>
+  <si>
+    <t>CaseApproval</t>
+  </si>
+  <si>
+    <t>QA_Automation_SmokeSuite27-Batch_01</t>
+  </si>
+  <si>
+    <t>QA_Auto20v15</t>
+  </si>
+  <si>
+    <t>QA_Auto20v15-Batch01</t>
   </si>
 </sst>
 </file>
@@ -923,7 +933,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -944,6 +954,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1233,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1613,34 +1624,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q168" workbookViewId="0">
-      <selection activeCell="W177" sqref="W177"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="E177" sqref="E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" customWidth="1"/>
     <col min="7" max="7" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.5703125" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" customWidth="1"/>
     <col min="10" max="10" width="28.42578125" customWidth="1"/>
     <col min="11" max="11" width="23.42578125" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
     <col min="13" max="13" width="21.85546875" customWidth="1"/>
     <col min="14" max="14" width="24.140625" customWidth="1"/>
-    <col min="15" max="15" width="23" customWidth="1"/>
+    <col min="15" max="15" width="30.85546875" customWidth="1"/>
     <col min="16" max="16" width="28.140625" customWidth="1"/>
     <col min="17" max="17" width="16.42578125" customWidth="1"/>
     <col min="18" max="18" width="22.85546875" customWidth="1"/>
     <col min="19" max="19" width="20.85546875" customWidth="1"/>
     <col min="20" max="20" width="19.140625" customWidth="1"/>
     <col min="21" max="21" width="16.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.140625" customWidth="1"/>
+    <col min="22" max="22" width="40.7109375" customWidth="1"/>
     <col min="23" max="23" width="24.140625" customWidth="1"/>
     <col min="24" max="24" width="18" customWidth="1"/>
     <col min="25" max="25" width="25.28515625" customWidth="1"/>
@@ -1908,10 +1919,10 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="18"/>
+      <c r="B21" s="19"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
@@ -1987,10 +1998,10 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="19"/>
+      <c r="B29" s="20"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
@@ -2027,11 +2038,11 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
@@ -2068,12 +2079,12 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
@@ -2110,12 +2121,12 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
@@ -2152,12 +2163,12 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
@@ -2212,12 +2223,12 @@
       </c>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="2" t="s">
@@ -2274,12 +2285,12 @@
       <c r="I51" s="7"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="2" t="s">
@@ -2346,12 +2357,12 @@
       </c>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="18" t="s">
+      <c r="A57" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="2" t="s">
@@ -2424,12 +2435,12 @@
       </c>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="2" t="s">
@@ -2484,12 +2495,12 @@
       </c>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="18"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="18"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="2" t="s">
@@ -2568,12 +2579,12 @@
       </c>
     </row>
     <row r="69" spans="1:12">
-      <c r="A69" s="18" t="s">
+      <c r="A69" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="2" t="s">
@@ -2634,12 +2645,12 @@
       </c>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="18" t="s">
+      <c r="A73" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="2" t="s">
@@ -2721,12 +2732,12 @@
       <c r="L76" s="7"/>
     </row>
     <row r="77" spans="1:12">
-      <c r="A77" s="18" t="s">
+      <c r="A77" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
-      <c r="D77" s="18"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="2" t="s">
@@ -2799,12 +2810,12 @@
       </c>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="18" t="s">
+      <c r="A81" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="18"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="2" t="s">
@@ -2871,12 +2882,12 @@
       </c>
     </row>
     <row r="85" spans="1:11">
-      <c r="A85" s="18" t="s">
+      <c r="A85" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B85" s="18"/>
-      <c r="C85" s="18"/>
-      <c r="D85" s="18"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="2" t="s">
@@ -2949,12 +2960,12 @@
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="A89" s="18" t="s">
+      <c r="A89" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B89" s="18"/>
-      <c r="C89" s="18"/>
-      <c r="D89" s="18"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
     </row>
     <row r="90" spans="1:11">
       <c r="A90" s="2" t="s">
@@ -3021,12 +3032,12 @@
       </c>
     </row>
     <row r="93" spans="1:11">
-      <c r="A93" s="18" t="s">
+      <c r="A93" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B93" s="18"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="18"/>
+      <c r="B93" s="19"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="19"/>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="2" t="s">
@@ -3087,12 +3098,12 @@
       </c>
     </row>
     <row r="97" spans="1:15">
-      <c r="A97" s="18" t="s">
+      <c r="A97" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
+      <c r="B97" s="19"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="19"/>
     </row>
     <row r="98" spans="1:15">
       <c r="A98" s="2" t="s">
@@ -3147,12 +3158,12 @@
       </c>
     </row>
     <row r="101" spans="1:15">
-      <c r="A101" s="18" t="s">
+      <c r="A101" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B101" s="18"/>
-      <c r="C101" s="18"/>
-      <c r="D101" s="18"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="19"/>
     </row>
     <row r="102" spans="1:15">
       <c r="A102" s="2" t="s">
@@ -3249,12 +3260,12 @@
       </c>
     </row>
     <row r="105" spans="1:15">
-      <c r="A105" s="18" t="s">
+      <c r="A105" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B105" s="18"/>
-      <c r="C105" s="18"/>
-      <c r="D105" s="18"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="19"/>
+      <c r="D105" s="19"/>
     </row>
     <row r="106" spans="1:15">
       <c r="A106" s="2" t="s">
@@ -3304,12 +3315,12 @@
       </c>
     </row>
     <row r="109" spans="1:15">
-      <c r="A109" s="18" t="s">
+      <c r="A109" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B109" s="18"/>
-      <c r="C109" s="18"/>
-      <c r="D109" s="18"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="19"/>
     </row>
     <row r="110" spans="1:15">
       <c r="A110" s="2" t="s">
@@ -3388,12 +3399,12 @@
       </c>
     </row>
     <row r="113" spans="1:13">
-      <c r="A113" s="18" t="s">
+      <c r="A113" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B113" s="18"/>
-      <c r="C113" s="18"/>
-      <c r="D113" s="18"/>
+      <c r="B113" s="19"/>
+      <c r="C113" s="19"/>
+      <c r="D113" s="19"/>
     </row>
     <row r="114" spans="1:13">
       <c r="A114" s="2" t="s">
@@ -3478,12 +3489,12 @@
       </c>
     </row>
     <row r="117" spans="1:13">
-      <c r="A117" s="18" t="s">
+      <c r="A117" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B117" s="18"/>
-      <c r="C117" s="18"/>
-      <c r="D117" s="18"/>
+      <c r="B117" s="19"/>
+      <c r="C117" s="19"/>
+      <c r="D117" s="19"/>
     </row>
     <row r="118" spans="1:13">
       <c r="A118" s="2" t="s">
@@ -3533,12 +3544,12 @@
       </c>
     </row>
     <row r="121" spans="1:13">
-      <c r="A121" s="18" t="s">
+      <c r="A121" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B121" s="18"/>
-      <c r="C121" s="18"/>
-      <c r="D121" s="18"/>
+      <c r="B121" s="19"/>
+      <c r="C121" s="19"/>
+      <c r="D121" s="19"/>
     </row>
     <row r="122" spans="1:13">
       <c r="A122" s="2" t="s">
@@ -3600,12 +3611,12 @@
       </c>
     </row>
     <row r="125" spans="1:13">
-      <c r="A125" s="18" t="s">
+      <c r="A125" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B125" s="18"/>
-      <c r="C125" s="18"/>
-      <c r="D125" s="18"/>
+      <c r="B125" s="19"/>
+      <c r="C125" s="19"/>
+      <c r="D125" s="19"/>
     </row>
     <row r="126" spans="1:13">
       <c r="A126" s="2" t="s">
@@ -3648,12 +3659,12 @@
       </c>
     </row>
     <row r="129" spans="1:13">
-      <c r="A129" s="18" t="s">
+      <c r="A129" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B129" s="18"/>
-      <c r="C129" s="18"/>
-      <c r="D129" s="18"/>
+      <c r="B129" s="19"/>
+      <c r="C129" s="19"/>
+      <c r="D129" s="19"/>
     </row>
     <row r="130" spans="1:13">
       <c r="A130" s="2" t="s">
@@ -3708,12 +3719,12 @@
       </c>
     </row>
     <row r="133" spans="1:13">
-      <c r="A133" s="18" t="s">
+      <c r="A133" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B133" s="18"/>
-      <c r="C133" s="18"/>
-      <c r="D133" s="18"/>
+      <c r="B133" s="19"/>
+      <c r="C133" s="19"/>
+      <c r="D133" s="19"/>
     </row>
     <row r="134" spans="1:13">
       <c r="A134" s="2" t="s">
@@ -3756,12 +3767,12 @@
       </c>
     </row>
     <row r="137" spans="1:13">
-      <c r="A137" s="18" t="s">
+      <c r="A137" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B137" s="18"/>
-      <c r="C137" s="18"/>
-      <c r="D137" s="18"/>
+      <c r="B137" s="19"/>
+      <c r="C137" s="19"/>
+      <c r="D137" s="19"/>
     </row>
     <row r="138" spans="1:13">
       <c r="A138" s="2" t="s">
@@ -3828,12 +3839,12 @@
       </c>
     </row>
     <row r="141" spans="1:13">
-      <c r="A141" s="18" t="s">
+      <c r="A141" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B141" s="18"/>
-      <c r="C141" s="18"/>
-      <c r="D141" s="18"/>
+      <c r="B141" s="19"/>
+      <c r="C141" s="19"/>
+      <c r="D141" s="19"/>
     </row>
     <row r="142" spans="1:13">
       <c r="A142" s="2" t="s">
@@ -3918,12 +3929,12 @@
       </c>
     </row>
     <row r="145" spans="1:21">
-      <c r="A145" s="18" t="s">
+      <c r="A145" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B145" s="18"/>
-      <c r="C145" s="18"/>
-      <c r="D145" s="18"/>
+      <c r="B145" s="19"/>
+      <c r="C145" s="19"/>
+      <c r="D145" s="19"/>
     </row>
     <row r="146" spans="1:21">
       <c r="A146" s="2" t="s">
@@ -4050,12 +4061,12 @@
       </c>
     </row>
     <row r="149" spans="1:21" ht="15" customHeight="1">
-      <c r="A149" s="18" t="s">
+      <c r="A149" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B149" s="18"/>
-      <c r="C149" s="18"/>
-      <c r="D149" s="18"/>
+      <c r="B149" s="19"/>
+      <c r="C149" s="19"/>
+      <c r="D149" s="19"/>
     </row>
     <row r="150" spans="1:21" ht="15" customHeight="1">
       <c r="A150" s="2" t="s">
@@ -4223,6 +4234,9 @@
       <c r="I154" t="s">
         <v>233</v>
       </c>
+      <c r="J154" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="155" spans="1:21" ht="15" customHeight="1">
       <c r="A155" t="s">
@@ -4241,25 +4255,28 @@
         <v>71</v>
       </c>
       <c r="F155" t="s">
-        <v>234</v>
-      </c>
-      <c r="G155" s="1" t="s">
         <v>235</v>
       </c>
+      <c r="G155" s="18" t="s">
+        <v>236</v>
+      </c>
       <c r="H155" t="s">
-        <v>163</v>
+        <v>237</v>
       </c>
       <c r="I155" t="s">
-        <v>236</v>
+        <v>238</v>
+      </c>
+      <c r="J155" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="157" spans="1:21" ht="15" customHeight="1">
-      <c r="A157" s="18" t="s">
+      <c r="A157" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B157" s="18"/>
-      <c r="C157" s="18"/>
-      <c r="D157" s="18"/>
+      <c r="B157" s="19"/>
+      <c r="C157" s="19"/>
+      <c r="D157" s="19"/>
     </row>
     <row r="158" spans="1:21" ht="15" customHeight="1">
       <c r="A158" s="2" t="s">
@@ -4343,7 +4360,7 @@
         <v>71</v>
       </c>
       <c r="F159" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G159" t="s">
         <v>205</v>
@@ -4355,7 +4372,7 @@
         <v>207</v>
       </c>
       <c r="J159" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="K159" t="s">
         <v>69</v>
@@ -4392,12 +4409,12 @@
       </c>
     </row>
     <row r="161" spans="1:28" ht="15" customHeight="1">
-      <c r="A161" s="18" t="s">
+      <c r="A161" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B161" s="18"/>
-      <c r="C161" s="18"/>
-      <c r="D161" s="18"/>
+      <c r="B161" s="19"/>
+      <c r="C161" s="19"/>
+      <c r="D161" s="19"/>
     </row>
     <row r="162" spans="1:28" ht="15" customHeight="1">
       <c r="A162" s="2" t="s">
@@ -4481,7 +4498,7 @@
         <v>71</v>
       </c>
       <c r="F163" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="G163" t="s">
         <v>205</v>
@@ -4493,7 +4510,7 @@
         <v>207</v>
       </c>
       <c r="J163" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="K163" t="s">
         <v>69</v>
@@ -4530,12 +4547,12 @@
       </c>
     </row>
     <row r="165" spans="1:28" ht="15" customHeight="1">
-      <c r="A165" s="18" t="s">
+      <c r="A165" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B165" s="18"/>
-      <c r="C165" s="18"/>
-      <c r="D165" s="18"/>
+      <c r="B165" s="19"/>
+      <c r="C165" s="19"/>
+      <c r="D165" s="19"/>
     </row>
     <row r="166" spans="1:28" ht="15" customHeight="1">
       <c r="A166" s="2" t="s">
@@ -4563,10 +4580,10 @@
         <v>147</v>
       </c>
       <c r="I166" s="11" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="J166" s="11" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="K166" s="11" t="s">
         <v>201</v>
@@ -4630,7 +4647,7 @@
         <v>71</v>
       </c>
       <c r="F167" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="G167" s="1" t="s">
         <v>88</v>
@@ -4639,10 +4656,10 @@
         <v>89</v>
       </c>
       <c r="I167" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="J167" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="K167" t="s">
         <v>205</v>
@@ -4654,13 +4671,13 @@
         <v>223</v>
       </c>
       <c r="N167" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="O167" t="s">
         <v>207</v>
       </c>
       <c r="P167" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="Q167" t="s">
         <v>69</v>
@@ -4736,7 +4753,7 @@
         <v>68</v>
       </c>
       <c r="O170" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="P170" t="s">
         <v>232</v>
@@ -4748,13 +4765,13 @@
         <v>158</v>
       </c>
       <c r="S170" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="T170" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="U170" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="V170" t="s">
         <v>186</v>
@@ -4767,11 +4784,11 @@
       <c r="B171" t="s">
         <v>51</v>
       </c>
-      <c r="C171" t="s">
-        <v>69</v>
+      <c r="C171" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D171" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E171" t="s">
         <v>71</v>
@@ -4783,7 +4800,7 @@
         <v>73</v>
       </c>
       <c r="H171" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="I171" t="s">
         <v>75</v>
@@ -4804,37 +4821,37 @@
         <v>79</v>
       </c>
       <c r="O171" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="P171" t="s">
-        <v>163</v>
+        <v>237</v>
       </c>
       <c r="Q171" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="R171" t="s">
-        <v>163</v>
+        <v>256</v>
       </c>
       <c r="S171" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="T171" t="s">
-        <v>223</v>
+        <v>258</v>
       </c>
       <c r="U171" s="17" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="V171" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="173" spans="1:28" ht="15" customHeight="1">
-      <c r="A173" s="18" t="s">
+      <c r="A173" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B173" s="18"/>
-      <c r="C173" s="18"/>
-      <c r="D173" s="18"/>
+      <c r="B173" s="19"/>
+      <c r="C173" s="19"/>
+      <c r="D173" s="19"/>
     </row>
     <row r="174" spans="1:28" ht="15" customHeight="1">
       <c r="A174" s="2" t="s">
@@ -4862,10 +4879,10 @@
         <v>147</v>
       </c>
       <c r="I174" s="11" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="J174" s="11" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="K174" s="11" t="s">
         <v>201</v>
@@ -4924,7 +4941,7 @@
         <v>71</v>
       </c>
       <c r="F175" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="G175" s="1" t="s">
         <v>88</v>
@@ -4933,10 +4950,10 @@
         <v>89</v>
       </c>
       <c r="I175" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="J175" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="K175" t="s">
         <v>205</v>
@@ -4948,13 +4965,13 @@
         <v>223</v>
       </c>
       <c r="N175" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="O175" t="s">
         <v>207</v>
       </c>
       <c r="P175" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="Q175" t="s">
         <v>69</v>
@@ -4980,23 +4997,12 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A173:D173"/>
-    <mergeCell ref="A165:D165"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="A133:D133"/>
-    <mergeCell ref="A129:D129"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A105:D105"/>
+    <mergeCell ref="A125:D125"/>
     <mergeCell ref="A101:D101"/>
     <mergeCell ref="A97:D97"/>
     <mergeCell ref="A113:D113"/>
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A117:D117"/>
-    <mergeCell ref="A137:D137"/>
-    <mergeCell ref="A141:D141"/>
     <mergeCell ref="A77:D77"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A41:D41"/>
@@ -5011,11 +5017,22 @@
     <mergeCell ref="A73:D73"/>
     <mergeCell ref="A69:D69"/>
     <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A173:D173"/>
     <mergeCell ref="A161:D161"/>
     <mergeCell ref="A157:D157"/>
     <mergeCell ref="A149:D149"/>
     <mergeCell ref="A145:D145"/>
-    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A165:D165"/>
+    <mergeCell ref="A137:D137"/>
+    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A133:D133"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A105:D105"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -5125,7 +5142,7 @@
     <hyperlink ref="C11" r:id="rId105" display="nmalegam@ligl.io" xr:uid="{ABF323FA-7B90-44C1-8D5D-F432051D88C3}"/>
     <hyperlink ref="D11" r:id="rId106" xr:uid="{ACEF8D99-DE27-42E2-AEC5-C396346ADBF4}"/>
     <hyperlink ref="G167" r:id="rId107" xr:uid="{7D2536A0-8BFC-42D6-AEC4-F0F3A31A42BB}"/>
-    <hyperlink ref="C171" r:id="rId108" display="nmalegam@ligl.io" xr:uid="{3700B464-823E-4A0A-9528-D30AE8439CBD}"/>
+    <hyperlink ref="C171" r:id="rId108" xr:uid="{3700B464-823E-4A0A-9528-D30AE8439CBD}"/>
     <hyperlink ref="D171" r:id="rId109" xr:uid="{20F8FD15-C039-4831-BA5B-4680F0BF4910}"/>
     <hyperlink ref="O171" r:id="rId110" xr:uid="{1D766624-AAD1-4778-A5B1-63769F263A0B}"/>
     <hyperlink ref="D175" r:id="rId111" xr:uid="{8A0956B6-D9D4-439E-ACA3-98967207D4AD}"/>
@@ -5140,17 +5157,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="dd3352ec-2343-4e5a-a362-ae5c8d10b401" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0749316b-3bc6-4054-b848-1af5bbc08270">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5159,7 +5165,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="दस्तावेज़" ma:contentTypeID="0x01010097E6DE5148608D42BEA665E616D802D4" ma:contentTypeVersion="17" ma:contentTypeDescription="कोई नया दस्‍तावेज़ बनाएँ." ma:contentTypeScope="" ma:versionID="5e0c99f15cbcbea0f31595d8f225d817">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0749316b-3bc6-4054-b848-1af5bbc08270" xmlns:ns3="dd3352ec-2343-4e5a-a362-ae5c8d10b401" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="256771933742ec89c8424a59e56826dd" ns2:_="" ns3:_="">
     <xsd:import namespace="0749316b-3bc6-4054-b848-1af5bbc08270"/>
@@ -5396,14 +5402,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dd3352ec-2343-4e5a-a362-ae5c8d10b401" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0749316b-3bc6-4054-b848-1af5bbc08270">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5236BF0A-7377-48E2-970B-AC3E69B99D6D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{442FA49D-68DF-49F1-BD4A-D57C699293AD}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{442FA49D-68DF-49F1-BD4A-D57C699293AD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{120226CC-2588-4AA6-A0B8-17FF0E8E0411}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{120226CC-2588-4AA6-A0B8-17FF0E8E0411}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5236BF0A-7377-48E2-970B-AC3E69B99D6D}"/>
 </file>
</xml_diff>

<commit_message>
User details and Entity moved to Properties file
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmalegam\Desktop\Reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE1DF3D-33F5-4452-8034-22E9E36D9038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4113302-8841-4C3A-8400-9BF3D80C8103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestStatus" sheetId="2" r:id="rId1"/>
     <sheet name="TestCases" sheetId="1" r:id="rId2"/>
+    <sheet name="MetaData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="328">
   <si>
     <t>TCID</t>
   </si>
@@ -1008,13 +1009,65 @@
     <t>LoginUser</t>
   </si>
   <si>
-    <t>superUSER</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Vertical.321</t>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>ssouser</t>
+  </si>
+  <si>
+    <t>In TestData Sheet</t>
+  </si>
+  <si>
+    <r>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should be Rel,EUR,Custom</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LoginUser</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should be ssouser, adminuser, superuser, customuser</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1362,7 +1415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1440,28 +1493,10 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1482,6 +1517,26 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1766,7 +1821,7 @@
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2570,7 +2625,7 @@
   <dimension ref="A1:FJ208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -2628,54 +2683,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1">
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="59"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1">
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
     </row>
     <row r="4" spans="1:10" ht="21" customHeight="1">
-      <c r="A4" s="70"/>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="68"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
     </row>
     <row r="6" spans="1:10" ht="14.25">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="59" t="s">
         <v>321</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
     </row>
     <row r="7" spans="1:10" ht="14.25">
       <c r="A7" s="2" t="s">
@@ -2684,64 +2739,54 @@
       <c r="B7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>65</v>
+      <c r="C7" s="8" t="s">
+        <v>322</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="E7" s="8" t="s">
+        <v>68</v>
+      </c>
       <c r="F7" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>322</v>
-      </c>
+      <c r="I7" s="71"/>
     </row>
     <row r="8" spans="1:10" ht="14.25">
-      <c r="A8" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="47" t="s">
+      <c r="A8" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="71" t="s">
         <v>324</v>
       </c>
-      <c r="D8" s="47" t="s">
-        <v>325</v>
-      </c>
-      <c r="E8" t="s">
-        <v>98</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="D8" s="71" t="s">
+        <v>323</v>
+      </c>
+      <c r="E8" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="I8" t="s">
-        <v>323</v>
-      </c>
+      <c r="I8" s="71"/>
     </row>
     <row r="10" spans="1:10" ht="14.25">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
     </row>
     <row r="11" spans="1:10" ht="14.25">
       <c r="A11" s="2" t="s">
@@ -2798,12 +2843,12 @@
       <c r="I12" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="14.25">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
     </row>
     <row r="15" spans="1:10" ht="14.25">
       <c r="A15" s="2" t="s">
@@ -2870,12 +2915,12 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="14.25">
-      <c r="A18" s="64" t="s">
+      <c r="A18" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
     </row>
     <row r="19" spans="1:12" ht="14.25">
       <c r="A19" s="2" t="s">
@@ -2948,12 +2993,12 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="14.25">
-      <c r="A22" s="64" t="s">
+      <c r="A22" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
     </row>
     <row r="23" spans="1:12" ht="14.25">
       <c r="A23" s="2" t="s">
@@ -3008,12 +3053,12 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="14.25">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
     </row>
     <row r="27" spans="1:12" ht="14.25">
       <c r="A27" s="2" t="s">
@@ -3092,12 +3137,12 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="14.25">
-      <c r="A30" s="64" t="s">
+      <c r="A30" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
     </row>
     <row r="31" spans="1:12" ht="14.25">
       <c r="A31" s="2" t="s">
@@ -3162,12 +3207,12 @@
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:15" ht="14.25">
-      <c r="A34" s="64" t="s">
+      <c r="A34" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="64"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
     </row>
     <row r="35" spans="1:15" ht="14.25">
       <c r="A35" s="2" t="s">
@@ -3268,12 +3313,12 @@
       <c r="H37" s="4"/>
     </row>
     <row r="39" spans="1:15" ht="14.25">
-      <c r="A39" s="64" t="s">
+      <c r="A39" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="64"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
     </row>
     <row r="40" spans="1:15" ht="14.25">
       <c r="A40" s="2" t="s">
@@ -3355,12 +3400,12 @@
       <c r="L42" s="4"/>
     </row>
     <row r="43" spans="1:15" ht="14.25">
-      <c r="A43" s="64" t="s">
+      <c r="A43" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="64"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
     </row>
     <row r="44" spans="1:15" ht="14.25">
       <c r="A44" s="2" t="s">
@@ -3433,12 +3478,12 @@
       </c>
     </row>
     <row r="47" spans="1:15" ht="14.25">
-      <c r="A47" s="64" t="s">
+      <c r="A47" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="64"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="64"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
     </row>
     <row r="48" spans="1:15" ht="14.25">
       <c r="A48" s="2" t="s">
@@ -3505,12 +3550,12 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="14.25">
-      <c r="A51" s="64" t="s">
+      <c r="A51" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="64"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
+      <c r="B51" s="57"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
     </row>
     <row r="52" spans="1:11" ht="14.25">
       <c r="A52" s="2" t="s">
@@ -3583,12 +3628,12 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="14.25">
-      <c r="A55" s="64" t="s">
+      <c r="A55" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="64"/>
-      <c r="C55" s="64"/>
-      <c r="D55" s="64"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
     </row>
     <row r="56" spans="1:11" ht="14.25">
       <c r="A56" s="2" t="s">
@@ -3655,12 +3700,12 @@
       </c>
     </row>
     <row r="59" spans="1:11" ht="14.25">
-      <c r="A59" s="64" t="s">
+      <c r="A59" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="64"/>
-      <c r="C59" s="64"/>
-      <c r="D59" s="64"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
     </row>
     <row r="60" spans="1:11" ht="14.25">
       <c r="A60" s="2" t="s">
@@ -3721,12 +3766,12 @@
       </c>
     </row>
     <row r="63" spans="1:11" ht="14.25">
-      <c r="A63" s="64" t="s">
+      <c r="A63" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B63" s="64"/>
-      <c r="C63" s="64"/>
-      <c r="D63" s="64"/>
+      <c r="B63" s="57"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="57"/>
     </row>
     <row r="64" spans="1:11" ht="14.25">
       <c r="A64" s="2" t="s">
@@ -3781,12 +3826,12 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="15" customHeight="1">
-      <c r="A67" s="64" t="s">
+      <c r="A67" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="B67" s="64"/>
-      <c r="C67" s="64"/>
-      <c r="D67" s="64"/>
+      <c r="B67" s="57"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="57"/>
     </row>
     <row r="68" spans="1:13" ht="15" customHeight="1">
       <c r="A68" s="2" t="s">
@@ -3847,12 +3892,12 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="15" customHeight="1">
-      <c r="A71" s="64" t="s">
+      <c r="A71" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B71" s="64"/>
-      <c r="C71" s="64"/>
-      <c r="D71" s="64"/>
+      <c r="B71" s="57"/>
+      <c r="C71" s="57"/>
+      <c r="D71" s="57"/>
     </row>
     <row r="72" spans="1:13" ht="15" customHeight="1">
       <c r="A72" s="2" t="s">
@@ -3895,12 +3940,12 @@
       </c>
     </row>
     <row r="75" spans="1:13" ht="14.25">
-      <c r="A75" s="64" t="s">
+      <c r="A75" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="B75" s="64"/>
-      <c r="C75" s="64"/>
-      <c r="D75" s="64"/>
+      <c r="B75" s="57"/>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57"/>
     </row>
     <row r="76" spans="1:13" ht="14.25">
       <c r="A76" s="2" t="s">
@@ -3950,12 +3995,12 @@
     </row>
     <row r="78" spans="1:13" ht="14.25"/>
     <row r="79" spans="1:13" ht="14.25">
-      <c r="A79" s="64" t="s">
+      <c r="A79" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B79" s="64"/>
-      <c r="C79" s="64"/>
-      <c r="D79" s="64"/>
+      <c r="B79" s="57"/>
+      <c r="C79" s="57"/>
+      <c r="D79" s="57"/>
     </row>
     <row r="80" spans="1:13" ht="14.25">
       <c r="A80" s="2" t="s">
@@ -4041,12 +4086,12 @@
     </row>
     <row r="82" spans="1:13" ht="14.25"/>
     <row r="83" spans="1:13" ht="14.25">
-      <c r="A83" s="64" t="s">
+      <c r="A83" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B83" s="64"/>
-      <c r="C83" s="64"/>
-      <c r="D83" s="64"/>
+      <c r="B83" s="57"/>
+      <c r="C83" s="57"/>
+      <c r="D83" s="57"/>
     </row>
     <row r="84" spans="1:13" ht="14.25">
       <c r="A84" s="2" t="s">
@@ -4126,12 +4171,12 @@
     </row>
     <row r="86" spans="1:13" ht="14.25"/>
     <row r="87" spans="1:13" ht="14.25">
-      <c r="A87" s="64" t="s">
+      <c r="A87" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B87" s="64"/>
-      <c r="C87" s="64"/>
-      <c r="D87" s="64"/>
+      <c r="B87" s="57"/>
+      <c r="C87" s="57"/>
+      <c r="D87" s="57"/>
     </row>
     <row r="88" spans="1:13" ht="14.25">
       <c r="A88" s="2" t="s">
@@ -4181,12 +4226,12 @@
     </row>
     <row r="90" spans="1:13" ht="14.25"/>
     <row r="91" spans="1:13" ht="14.25">
-      <c r="A91" s="64" t="s">
+      <c r="A91" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B91" s="64"/>
-      <c r="C91" s="64"/>
-      <c r="D91" s="64"/>
+      <c r="B91" s="57"/>
+      <c r="C91" s="57"/>
+      <c r="D91" s="57"/>
     </row>
     <row r="92" spans="1:13" ht="14.25">
       <c r="A92" s="2" t="s">
@@ -4254,12 +4299,12 @@
     </row>
     <row r="94" spans="1:13" ht="14.25"/>
     <row r="95" spans="1:13" ht="14.25">
-      <c r="A95" s="64" t="s">
+      <c r="A95" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B95" s="64"/>
-      <c r="C95" s="64"/>
-      <c r="D95" s="64"/>
+      <c r="B95" s="57"/>
+      <c r="C95" s="57"/>
+      <c r="D95" s="57"/>
     </row>
     <row r="96" spans="1:13" ht="14.25">
       <c r="A96" s="2" t="s">
@@ -4303,12 +4348,12 @@
     </row>
     <row r="98" spans="1:20" ht="14.25"/>
     <row r="99" spans="1:20" ht="14.25">
-      <c r="A99" s="64" t="s">
+      <c r="A99" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B99" s="64"/>
-      <c r="C99" s="64"/>
-      <c r="D99" s="64"/>
+      <c r="B99" s="57"/>
+      <c r="C99" s="57"/>
+      <c r="D99" s="57"/>
     </row>
     <row r="100" spans="1:20" ht="14.25">
       <c r="A100" s="2" t="s">
@@ -4364,12 +4409,12 @@
     </row>
     <row r="102" spans="1:20" ht="14.25"/>
     <row r="103" spans="1:20" ht="14.25">
-      <c r="A103" s="64" t="s">
+      <c r="A103" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="B103" s="64"/>
-      <c r="C103" s="64"/>
-      <c r="D103" s="64"/>
+      <c r="B103" s="57"/>
+      <c r="C103" s="57"/>
+      <c r="D103" s="57"/>
     </row>
     <row r="104" spans="1:20" ht="14.25">
       <c r="A104" s="2" t="s">
@@ -4455,28 +4500,28 @@
     </row>
     <row r="106" spans="1:20" ht="14.25"/>
     <row r="107" spans="1:20" ht="14.25">
-      <c r="A107" s="57" t="s">
+      <c r="A107" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="B107" s="58"/>
-      <c r="C107" s="58"/>
-      <c r="D107" s="58"/>
+      <c r="B107" s="66"/>
+      <c r="C107" s="66"/>
+      <c r="D107" s="66"/>
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="1:20" ht="14.25">
-      <c r="A108" s="58"/>
-      <c r="B108" s="58"/>
-      <c r="C108" s="58"/>
-      <c r="D108" s="58"/>
+      <c r="A108" s="66"/>
+      <c r="B108" s="66"/>
+      <c r="C108" s="66"/>
+      <c r="D108" s="66"/>
       <c r="G108" s="1"/>
     </row>
     <row r="110" spans="1:20" ht="14.25">
-      <c r="A110" s="62" t="s">
+      <c r="A110" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B110" s="62"/>
-      <c r="C110" s="62"/>
-      <c r="D110" s="62"/>
+      <c r="B110" s="58"/>
+      <c r="C110" s="58"/>
+      <c r="D110" s="58"/>
     </row>
     <row r="111" spans="1:20" ht="14.25">
       <c r="A111" s="12" t="s">
@@ -4603,12 +4648,12 @@
       </c>
     </row>
     <row r="114" spans="1:23" ht="15" customHeight="1">
-      <c r="A114" s="62" t="s">
+      <c r="A114" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="B114" s="62"/>
-      <c r="C114" s="62"/>
-      <c r="D114" s="62"/>
+      <c r="B114" s="58"/>
+      <c r="C114" s="58"/>
+      <c r="D114" s="58"/>
     </row>
     <row r="115" spans="1:23" ht="15" customHeight="1">
       <c r="A115" s="12" t="s">
@@ -4744,12 +4789,12 @@
       <c r="P117" s="1"/>
     </row>
     <row r="118" spans="1:23" ht="15" customHeight="1">
-      <c r="A118" s="62" t="s">
+      <c r="A118" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B118" s="62"/>
-      <c r="C118" s="62"/>
-      <c r="D118" s="62"/>
+      <c r="B118" s="58"/>
+      <c r="C118" s="58"/>
+      <c r="D118" s="58"/>
     </row>
     <row r="119" spans="1:23" ht="15" customHeight="1">
       <c r="A119" s="12" t="s">
@@ -4882,12 +4927,12 @@
       </c>
     </row>
     <row r="122" spans="1:23" ht="15" customHeight="1">
-      <c r="A122" s="62" t="s">
+      <c r="A122" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="B122" s="62"/>
-      <c r="C122" s="62"/>
-      <c r="D122" s="62"/>
+      <c r="B122" s="58"/>
+      <c r="C122" s="58"/>
+      <c r="D122" s="58"/>
     </row>
     <row r="123" spans="1:23" ht="15" customHeight="1">
       <c r="A123" s="12" t="s">
@@ -5020,12 +5065,12 @@
       </c>
     </row>
     <row r="126" spans="1:23" ht="15" customHeight="1">
-      <c r="A126" s="62" t="s">
+      <c r="A126" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="B126" s="62"/>
-      <c r="C126" s="62"/>
-      <c r="D126" s="62"/>
+      <c r="B126" s="58"/>
+      <c r="C126" s="58"/>
+      <c r="D126" s="58"/>
     </row>
     <row r="127" spans="1:23" ht="15" customHeight="1">
       <c r="A127" s="12" t="s">
@@ -5173,12 +5218,12 @@
       <c r="P129" s="1"/>
     </row>
     <row r="130" spans="1:32" ht="15" customHeight="1">
-      <c r="A130" s="62" t="s">
+      <c r="A130" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B130" s="62"/>
-      <c r="C130" s="62"/>
-      <c r="D130" s="62"/>
+      <c r="B130" s="58"/>
+      <c r="C130" s="58"/>
+      <c r="D130" s="58"/>
     </row>
     <row r="131" spans="1:32" ht="15" customHeight="1">
       <c r="A131" s="12" t="s">
@@ -5323,12 +5368,12 @@
       </c>
     </row>
     <row r="134" spans="1:32" ht="15" customHeight="1">
-      <c r="A134" s="62" t="s">
+      <c r="A134" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B134" s="62"/>
-      <c r="C134" s="62"/>
-      <c r="D134" s="62"/>
+      <c r="B134" s="58"/>
+      <c r="C134" s="58"/>
+      <c r="D134" s="58"/>
     </row>
     <row r="135" spans="1:32" ht="15" customHeight="1">
       <c r="A135" s="12" t="s">
@@ -5468,12 +5513,12 @@
       </c>
     </row>
     <row r="138" spans="1:32" ht="15" customHeight="1">
-      <c r="A138" s="62" t="s">
+      <c r="A138" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="B138" s="62"/>
-      <c r="C138" s="62"/>
-      <c r="D138" s="62"/>
+      <c r="B138" s="58"/>
+      <c r="C138" s="58"/>
+      <c r="D138" s="58"/>
     </row>
     <row r="139" spans="1:32" ht="15" customHeight="1">
       <c r="A139" s="12" t="s">
@@ -5669,12 +5714,12 @@
       <c r="P141" s="1"/>
     </row>
     <row r="142" spans="1:32" ht="15" customHeight="1">
-      <c r="A142" s="62" t="s">
+      <c r="A142" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="B142" s="62"/>
-      <c r="C142" s="62"/>
-      <c r="D142" s="62"/>
+      <c r="B142" s="58"/>
+      <c r="C142" s="58"/>
+      <c r="D142" s="58"/>
     </row>
     <row r="143" spans="1:32" ht="15" customHeight="1">
       <c r="A143" s="12" t="s">
@@ -5873,12 +5918,12 @@
       </c>
     </row>
     <row r="146" spans="1:32" ht="15" customHeight="1">
-      <c r="A146" s="62" t="s">
+      <c r="A146" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B146" s="62"/>
-      <c r="C146" s="62"/>
-      <c r="D146" s="62"/>
+      <c r="B146" s="58"/>
+      <c r="C146" s="58"/>
+      <c r="D146" s="58"/>
     </row>
     <row r="147" spans="1:32" ht="15" customHeight="1">
       <c r="A147" s="12" t="s">
@@ -6077,12 +6122,12 @@
       </c>
     </row>
     <row r="150" spans="1:32" ht="15" customHeight="1">
-      <c r="A150" s="62" t="s">
+      <c r="A150" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B150" s="62"/>
-      <c r="C150" s="62"/>
-      <c r="D150" s="62"/>
+      <c r="B150" s="58"/>
+      <c r="C150" s="58"/>
+      <c r="D150" s="58"/>
     </row>
     <row r="151" spans="1:32" ht="15" customHeight="1">
       <c r="A151" s="12" t="s">
@@ -6281,35 +6326,35 @@
       </c>
     </row>
     <row r="153" spans="1:32" ht="15" customHeight="1">
-      <c r="A153" s="63"/>
-      <c r="B153" s="63"/>
-      <c r="C153" s="63"/>
-      <c r="D153" s="63"/>
-      <c r="E153" s="63"/>
-      <c r="F153" s="63"/>
-      <c r="G153" s="63"/>
-      <c r="H153" s="63"/>
+      <c r="A153" s="70"/>
+      <c r="B153" s="70"/>
+      <c r="C153" s="70"/>
+      <c r="D153" s="70"/>
+      <c r="E153" s="70"/>
+      <c r="F153" s="70"/>
+      <c r="G153" s="70"/>
+      <c r="H153" s="70"/>
       <c r="P153" s="1"/>
     </row>
     <row r="155" spans="1:32" ht="15" customHeight="1">
-      <c r="A155" s="60" t="s">
+      <c r="A155" s="68" t="s">
         <v>269</v>
       </c>
-      <c r="B155" s="61"/>
-      <c r="C155" s="61"/>
-      <c r="D155" s="61"/>
-      <c r="E155" s="61"/>
-      <c r="F155" s="61"/>
-      <c r="G155" s="61"/>
+      <c r="B155" s="69"/>
+      <c r="C155" s="69"/>
+      <c r="D155" s="69"/>
+      <c r="E155" s="69"/>
+      <c r="F155" s="69"/>
+      <c r="G155" s="69"/>
     </row>
     <row r="156" spans="1:32" ht="15" customHeight="1">
-      <c r="A156" s="61"/>
-      <c r="B156" s="61"/>
-      <c r="C156" s="61"/>
-      <c r="D156" s="61"/>
-      <c r="E156" s="61"/>
-      <c r="F156" s="61"/>
-      <c r="G156" s="61"/>
+      <c r="A156" s="69"/>
+      <c r="B156" s="69"/>
+      <c r="C156" s="69"/>
+      <c r="D156" s="69"/>
+      <c r="E156" s="69"/>
+      <c r="F156" s="69"/>
+      <c r="G156" s="69"/>
     </row>
     <row r="157" spans="1:32" ht="15" customHeight="1">
       <c r="A157" s="29"/>
@@ -8234,32 +8279,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A103:D103"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A130:D130"/>
-    <mergeCell ref="A122:D122"/>
-    <mergeCell ref="A118:D118"/>
-    <mergeCell ref="A114:D114"/>
-    <mergeCell ref="A110:D110"/>
-    <mergeCell ref="A126:D126"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A3:H4"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A95:D95"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A91:D91"/>
     <mergeCell ref="A107:D108"/>
     <mergeCell ref="E1:F2"/>
     <mergeCell ref="A155:G156"/>
@@ -8276,9 +8295,35 @@
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A3:H4"/>
+    <mergeCell ref="A130:D130"/>
+    <mergeCell ref="A122:D122"/>
+    <mergeCell ref="A118:D118"/>
+    <mergeCell ref="A114:D114"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="A126:D126"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A67:D67"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G8" r:id="rId1" xr:uid="{59BF35D7-2864-481F-8824-1D4A63D60F4F}"/>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{59BF35D7-2864-481F-8824-1D4A63D60F4F}"/>
     <hyperlink ref="G49" r:id="rId2" xr:uid="{45E704F1-3B24-4D88-8B7F-EC59044D167C}"/>
     <hyperlink ref="G65" r:id="rId3" xr:uid="{41FF77C7-FAE8-49BA-AA59-2B920E514817}"/>
     <hyperlink ref="G57" r:id="rId4" xr:uid="{32314F7E-35B0-496D-8B63-01A4D3FDF235}"/>
@@ -8417,23 +8462,53 @@
     <hyperlink ref="C93" r:id="rId137" display="nmalegam@ligl.io" xr:uid="{7E88CB7E-AF73-4162-8201-D548C931EF68}"/>
     <hyperlink ref="D208" r:id="rId138" xr:uid="{1937518B-DB9C-443A-8E4E-A8073AD0C42E}"/>
     <hyperlink ref="C208" r:id="rId139" xr:uid="{1736289C-501D-49D4-B8FB-29BE28A5961D}"/>
-    <hyperlink ref="D8" r:id="rId140" display="Vertical@123" xr:uid="{D7A7C3B8-6C30-4D00-9733-5F184517CF3A}"/>
-    <hyperlink ref="C8" r:id="rId141" display="nmalegam@ligl.io" xr:uid="{646F8B5D-BB99-4A38-8C8D-62E48F552274}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId142"/>
+  <pageSetup orientation="portrait" r:id="rId140"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2EEFC60-FD5D-4F6E-BC5F-397D2A3CD989}">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="54.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" s="72" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="dd3352ec-2343-4e5a-a362-ae5c8d10b401" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0749316b-3bc6-4054-b848-1af5bbc08270">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8674,21 +8749,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dd3352ec-2343-4e5a-a362-ae5c8d10b401" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0749316b-3bc6-4054-b848-1af5bbc08270">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5236BF0A-7377-48E2-970B-AC3E69B99D6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{442FA49D-68DF-49F1-BD4A-D57C699293AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dd3352ec-2343-4e5a-a362-ae5c8d10b401"/>
-    <ds:schemaRef ds:uri="0749316b-3bc6-4054-b848-1af5bbc08270"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8713,9 +8787,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{442FA49D-68DF-49F1-BD4A-D57C699293AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5236BF0A-7377-48E2-970B-AC3E69B99D6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dd3352ec-2343-4e5a-a362-ae5c8d10b401"/>
+    <ds:schemaRef ds:uri="0749316b-3bc6-4054-b848-1af5bbc08270"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>